<commit_message>
ajout incertitude sur la pente
</commit_message>
<xml_diff>
--- a/data/data045.xlsx
+++ b/data/data045.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Dev\Projets\phys_exp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD7C2A9-1707-4056-BCF0-F741C930ED69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48AF4E7-53A7-4878-A79A-999478F33218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1FBBF141-2BD8-47F5-A829-7AD7FC6B171A}"/>
   </bookViews>
@@ -399,7 +399,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -420,11 +420,9 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B2">
-        <f>6*10^-4</f>
-        <v>6.0000000000000006E-4</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C8" ca="1" si="0" xml:space="preserve"> 1.75*10^-8 * A2 /$C$2</f>
         <v>5.5016523537939125E-4</v>
       </c>
     </row>
@@ -433,11 +431,9 @@
         <v>0.01</v>
       </c>
       <c r="B3">
-        <f>1.5*10^-3</f>
         <v>1.5E-3</v>
       </c>
       <c r="C3">
-        <f t="shared" ca="1" si="0"/>
         <v>1.1003304707587825E-3</v>
       </c>
     </row>
@@ -446,11 +442,9 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="B4">
-        <f>2*10^-3</f>
         <v>2E-3</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
         <v>1.6504957061381736E-3</v>
       </c>
     </row>
@@ -459,11 +453,9 @@
         <v>0.02</v>
       </c>
       <c r="B5">
-        <f>27*10^-4</f>
         <v>2.7000000000000001E-3</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="0"/>
         <v>2.200660941517565E-3</v>
       </c>
     </row>
@@ -475,7 +467,6 @@
         <v>3.2000000000000002E-3</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="0"/>
         <v>2.7508261768969559E-3</v>
       </c>
     </row>
@@ -487,7 +478,6 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
         <v>3.3009914122763473E-3</v>
       </c>
     </row>
@@ -499,7 +489,6 @@
         <v>4.3E-3</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
         <v>3.851156647655739E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajout petites modifs data readme et gitignore
</commit_message>
<xml_diff>
--- a/data/data045.xlsx
+++ b/data/data045.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Dev\Projets\phys_exp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48AF4E7-53A7-4878-A79A-999478F33218}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA3DE36-E982-4DF9-8CD7-73D80E9FDD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1FBBF141-2BD8-47F5-A829-7AD7FC6B171A}"/>
+    <workbookView xWindow="9492" yWindow="0" windowWidth="11232" windowHeight="8520" xr2:uid="{1FBBF141-2BD8-47F5-A829-7AD7FC6B171A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Longueur</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Resistance</t>
+  </si>
+  <si>
+    <t>Resistance-</t>
   </si>
 </sst>
 </file>
@@ -396,15 +399,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F1369B-5EB5-45FE-8EEB-B700D51EFB74}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,8 +417,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>5.0000000000000001E-3</v>
       </c>
@@ -425,8 +431,12 @@
       <c r="C2">
         <v>5.5016523537939125E-4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2">
+        <f>B2-0.000428</f>
+        <v>6.7200000000000007E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0.01</v>
       </c>
@@ -436,8 +446,12 @@
       <c r="C3">
         <v>1.1003304707587825E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <f t="shared" ref="D3:D8" si="0">B3-0.000428</f>
+        <v>1.072E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1.4999999999999999E-2</v>
       </c>
@@ -447,8 +461,12 @@
       <c r="C4">
         <v>1.6504957061381736E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1.572E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.02</v>
       </c>
@@ -458,8 +476,12 @@
       <c r="C5">
         <v>2.200660941517565E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2.2720000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -469,8 +491,12 @@
       <c r="C6">
         <v>2.7508261768969559E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2.7720000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0.03</v>
       </c>
@@ -480,8 +506,12 @@
       <c r="C7">
         <v>3.3009914122763473E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>3.5720000000000001E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3.5000000000000003E-2</v>
       </c>
@@ -490,6 +520,10 @@
       </c>
       <c r="C8">
         <v>3.851156647655739E-3</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3.872E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>